<commit_message>
them bieu do vao trang thong ke
</commit_message>
<xml_diff>
--- a/Database_v2.xlsx
+++ b/Database_v2.xlsx
@@ -1145,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
chinh sua database, them module thong ke cua Hoai, can phai sua
</commit_message>
<xml_diff>
--- a/Database_v2.xlsx
+++ b/Database_v2.xlsx
@@ -111,8 +111,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">(cần phải + với lượng kalo cho hoạt động hằng ngày)
-</t>
+          <t xml:space="preserve">
+= tổng sum(luongkalotieuhao) from THONGKEBAITAP</t>
         </r>
       </text>
     </comment>
@@ -126,17 +126,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>ăn</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
+          <t>nhập từ thực đơn..
+Nếu không nhập = muctieu.chisobmr</t>
         </r>
       </text>
     </comment>
@@ -150,17 +141,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>+Lượng kalo khi tập
-+lượng kalo cho hoạt động hằng ngày</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">+Lượng kalo khi tập bài tập đó
 </t>
         </r>
       </text>
@@ -1146,7 +1127,7 @@
   <dimension ref="B2:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>